<commit_message>
Poprawione liczby i słowa bez powtórzeń
</commit_message>
<xml_diff>
--- a/Database_stats.xlsx
+++ b/Database_stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Dane statystyczne: Database.txt</t>
   </si>
@@ -215,13 +215,10 @@
     <t>czego</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>profesor</t>
+  </si>
+  <si>
+    <t>uczy</t>
   </si>
 </sst>
 </file>
@@ -279,7 +276,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -303,7 +300,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>371.0</v>
+        <v>365.0</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -317,13 +314,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>75.0</v>
+        <v>86.0</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>67</v>
+      <c r="D3" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -336,8 +333,8 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>68</v>
+      <c r="D4" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
@@ -350,8 +347,8 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>69</v>
+      <c r="D5" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -364,7 +361,9 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6"/>
+      <c r="D6" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -376,19 +375,23 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7"/>
+      <c r="D7" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>52.0</v>
+        <v>46.0</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8"/>
+      <c r="D8" t="n">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -400,7 +403,9 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9"/>
+      <c r="D9" t="n">
+        <v>9.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -412,7 +417,9 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D10"/>
+      <c r="D10" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11"/>
@@ -420,7 +427,9 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11"/>
+      <c r="D11" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12"/>
@@ -789,6 +798,22 @@
         <v>66</v>
       </c>
       <c r="D57"/>
+    </row>
+    <row r="58">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58"/>
+    </row>
+    <row r="59">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>

<commit_message>
Polskie znaki w excelu z readera #kozak
</commit_message>
<xml_diff>
--- a/Database_stats.xlsx
+++ b/Database_stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Dane statystyczne: Database.txt</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Cyfry bez powtórzeń</t>
   </si>
   <si>
-    <t>Zacz</t>
+    <t>Zaczął</t>
   </si>
   <si>
     <t>Pan</t>
@@ -59,31 +59,25 @@
     <t>nam</t>
   </si>
   <si>
-    <t>podsuwa</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>ne</t>
+    <t>podsuwać</t>
+  </si>
+  <si>
+    <t>różne</t>
   </si>
   <si>
     <t>lektury</t>
   </si>
   <si>
-    <t>kt</t>
-  </si>
-  <si>
-    <t>re</t>
-  </si>
-  <si>
-    <t>maj</t>
+    <t>które</t>
+  </si>
+  <si>
+    <t>mają</t>
   </si>
   <si>
     <t>nas</t>
   </si>
   <si>
-    <t>rozwija</t>
+    <t>rozwijać</t>
   </si>
   <si>
     <t>w</t>
@@ -98,7 +92,7 @@
     <t>mnie</t>
   </si>
   <si>
-    <t>jak</t>
+    <t>jaką</t>
   </si>
   <si>
     <t>opinie</t>
@@ -122,19 +116,13 @@
     <t>damsko</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>skich</t>
+    <t>męskich</t>
   </si>
   <si>
     <t>czy</t>
   </si>
   <si>
-    <t>jeste</t>
-  </si>
-  <si>
-    <t>my</t>
+    <t>jesteśmy</t>
   </si>
   <si>
     <t>odpowiednim</t>
@@ -146,28 +134,22 @@
     <t>do</t>
   </si>
   <si>
-    <t>anga</t>
-  </si>
-  <si>
-    <t>owania</t>
-  </si>
-  <si>
-    <t>si</t>
-  </si>
-  <si>
-    <t>zwi</t>
-  </si>
-  <si>
-    <t>zki</t>
+    <t>angażowania</t>
+  </si>
+  <si>
+    <t>się</t>
+  </si>
+  <si>
+    <t>związki</t>
   </si>
   <si>
     <t>Nie</t>
   </si>
   <si>
-    <t>powinni</t>
-  </si>
-  <si>
-    <t>skupi</t>
+    <t>powinniśmy</t>
+  </si>
+  <si>
+    <t>skupić</t>
   </si>
   <si>
     <t>naszym</t>
@@ -176,7 +158,7 @@
     <t>rozwoju</t>
   </si>
   <si>
-    <t>Przecie</t>
+    <t>Przecież</t>
   </si>
   <si>
     <t>inwestowanie</t>
@@ -185,7 +167,7 @@
     <t>czasu</t>
   </si>
   <si>
-    <t>kogo</t>
+    <t>kogoś</t>
   </si>
   <si>
     <t>z</t>
@@ -197,7 +179,7 @@
     <t>zapewne</t>
   </si>
   <si>
-    <t>kiedy</t>
+    <t>kiedyś</t>
   </si>
   <si>
     <t>rozstaniemy</t>
@@ -276,7 +258,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -300,7 +282,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>365.0</v>
+        <v>367.0</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -356,7 +338,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>286.0</v>
+        <v>310.0</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -398,7 +380,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>68.0</v>
+        <v>60.0</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -766,54 +748,6 @@
         <v>62</v>
       </c>
       <c r="D53"/>
-    </row>
-    <row r="54">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54"/>
-    </row>
-    <row r="55">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55"/>
-    </row>
-    <row r="56">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D56"/>
-    </row>
-    <row r="57">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57"/>
-    </row>
-    <row r="58">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58"/>
-    </row>
-    <row r="59">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59" t="s">
-        <v>68</v>
-      </c>
-      <c r="D59"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>